<commit_message>
Fixed calcmem for RobinHoodHashing
</commit_message>
<xml_diff>
--- a/MemoryCalcsUpdated.xlsx
+++ b/MemoryCalcsUpdated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucy-my.sharepoint.com/personal/ctheop03_ucy_ac_cy/Documents/Semesters/Third/EPL 231/231Dictionary-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{F8AF4A89-7181-4396-97B8-05524F43F88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88B817D0-522C-44E7-BE2F-AA8F100E4E78}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{F8AF4A89-7181-4396-97B8-05524F43F88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93F304A9-8925-411C-84ED-D5F2FE935C54}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1416" yWindow="744" windowWidth="21624" windowHeight="11112" xr2:uid="{D5927F62-1B0C-4F33-A786-18C4B429BD40}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5927F62-1B0C-4F33-A786-18C4B429BD40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3432,22 +3432,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>335412</c:v>
+                  <c:v>336512</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3302376</c:v>
+                  <c:v>3305852</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12803956</c:v>
+                  <c:v>12807388</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>155664388</c:v>
+                  <c:v>155670768</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>777564656</c:v>
+                  <c:v>777563952</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1828465716</c:v>
+                  <c:v>1828512312</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3519,22 +3519,22 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>177346</c:v>
+                  <c:v>76450</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1707089.2</c:v>
+                  <c:v>751310</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6530642</c:v>
+                  <c:v>2910880</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78805249.200000003</c:v>
+                  <c:v>35380090</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>392535543.60000002</c:v>
+                  <c:v>176721340</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>919345102.79999995</c:v>
+                  <c:v>415576480</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3887,22 +3887,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2266484</c:v>
+                  <c:v>2235288</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10706212</c:v>
+                  <c:v>10744272</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20968640</c:v>
+                  <c:v>21028656</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>194528884</c:v>
+                  <c:v>194553744</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>566258352</c:v>
+                  <c:v>566745124</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>930693148</c:v>
+                  <c:v>929866696</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3974,22 +3974,22 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1143045.6000000001</c:v>
+                  <c:v>507990</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5408954</c:v>
+                  <c:v>2441890</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10613027.199999999</c:v>
+                  <c:v>4779220</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98024020.799999997</c:v>
+                  <c:v>44217150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>286469689.19999999</c:v>
+                  <c:v>128807440</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>469954071.60000002</c:v>
+                  <c:v>211336920</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5724,8 +5724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F54434-1C8B-48AB-8957-A3893CADCD4A}">
   <dimension ref="B2:O1026"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M63" sqref="M63"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5828,46 +5828,46 @@
         <v>1000</v>
       </c>
       <c r="C4" s="6">
-        <v>2304940</v>
+        <v>2196480</v>
       </c>
       <c r="D4" s="7">
-        <v>1162632</v>
+        <v>499170</v>
       </c>
       <c r="E4" s="6">
-        <v>2382160</v>
+        <v>2197140</v>
       </c>
       <c r="F4" s="7">
-        <v>1200890</v>
+        <v>499320</v>
       </c>
       <c r="G4" s="6">
-        <v>2196480</v>
+        <v>2250380</v>
       </c>
       <c r="H4" s="7">
-        <v>1107666</v>
+        <v>511420</v>
       </c>
       <c r="I4" s="6">
-        <v>2212760</v>
+        <v>2309560</v>
       </c>
       <c r="J4" s="7">
-        <v>1116030</v>
+        <v>524870</v>
       </c>
       <c r="K4" s="6">
-        <v>2236080</v>
+        <v>2222880</v>
       </c>
       <c r="L4" s="7">
-        <v>1128010</v>
+        <v>505170</v>
       </c>
       <c r="M4" s="6">
         <f>AVERAGE(C4,E4,G4,I4,K4)</f>
-        <v>2266484</v>
+        <v>2235288</v>
       </c>
       <c r="N4" s="8">
         <f>AVERAGE(D4,F4,H4,J4,L4)</f>
-        <v>1143045.6000000001</v>
+        <v>507990</v>
       </c>
       <c r="O4" s="3">
         <f>M4/N4</f>
-        <v>1.9828465286074324</v>
+        <v>4.4002598476347963</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
@@ -5875,46 +5875,46 @@
         <v>5000</v>
       </c>
       <c r="C5" s="6">
-        <v>10939720</v>
+        <v>10804200</v>
       </c>
       <c r="D5" s="7">
-        <v>5525892</v>
+        <v>2455520</v>
       </c>
       <c r="E5" s="6">
-        <v>10555380</v>
+        <v>10980640</v>
       </c>
       <c r="F5" s="7">
-        <v>5334060</v>
+        <v>2495570</v>
       </c>
       <c r="G5" s="6">
-        <v>10584640</v>
+        <v>10806620</v>
       </c>
       <c r="H5" s="7">
-        <v>5347154</v>
+        <v>2456170</v>
       </c>
       <c r="I5" s="6">
-        <v>10805080</v>
+        <v>10602900</v>
       </c>
       <c r="J5" s="7">
-        <v>5458974</v>
+        <v>2409720</v>
       </c>
       <c r="K5" s="6">
-        <v>10646240</v>
+        <v>10527000</v>
       </c>
       <c r="L5" s="7">
-        <v>5378690</v>
+        <v>2392470</v>
       </c>
       <c r="M5" s="6">
         <f t="shared" ref="M5:M8" si="0">AVERAGE(C5,E5,G5,I5,K5)</f>
-        <v>10706212</v>
+        <v>10744272</v>
       </c>
       <c r="N5" s="8">
         <f>AVERAGE(D5,F5,H5,J5,L5)</f>
-        <v>5408954</v>
+        <v>2441890</v>
       </c>
       <c r="O5" s="3">
         <f t="shared" ref="O5:O9" si="1">M5/N5</f>
-        <v>1.979349796651996</v>
+        <v>4.3999819811703231</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
@@ -5922,46 +5922,46 @@
         <v>10000</v>
       </c>
       <c r="C6" s="6">
-        <v>20576820</v>
+        <v>20887900</v>
       </c>
       <c r="D6" s="7">
-        <v>10416864</v>
+        <v>4747220</v>
       </c>
       <c r="E6" s="6">
-        <v>21059940</v>
+        <v>21405780</v>
       </c>
       <c r="F6" s="7">
-        <v>10659584</v>
+        <v>4864970</v>
       </c>
       <c r="G6" s="6">
-        <v>20940040</v>
+        <v>20948180</v>
       </c>
       <c r="H6" s="7">
-        <v>10597760</v>
+        <v>4760920</v>
       </c>
       <c r="I6" s="6">
-        <v>21194360</v>
+        <v>20834660</v>
       </c>
       <c r="J6" s="7">
-        <v>10726954</v>
+        <v>4735120</v>
       </c>
       <c r="K6" s="6">
-        <v>21072040</v>
+        <v>21066760</v>
       </c>
       <c r="L6" s="7">
-        <v>10663974</v>
+        <v>4787870</v>
       </c>
       <c r="M6" s="6">
         <f t="shared" si="0"/>
-        <v>20968640</v>
+        <v>21028656</v>
       </c>
       <c r="N6" s="8">
         <f>AVERAGE(D6,F6,H6,J6,L6)</f>
-        <v>10613027.199999999</v>
+        <v>4779220</v>
       </c>
       <c r="O6" s="3">
         <f t="shared" si="1"/>
-        <v>1.9757454310491169</v>
+        <v>4.4000184130464808</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
@@ -5969,46 +5969,46 @@
         <v>100000</v>
       </c>
       <c r="C7" s="6">
-        <v>194520920</v>
+        <v>194067500</v>
       </c>
       <c r="D7" s="7">
-        <v>98024786</v>
+        <v>44106320</v>
       </c>
       <c r="E7" s="6">
-        <v>194685700</v>
+        <v>195299500</v>
       </c>
       <c r="F7" s="7">
-        <v>98105726</v>
+        <v>44386670</v>
       </c>
       <c r="G7" s="6">
-        <v>193736840</v>
+        <v>194030980</v>
       </c>
       <c r="H7" s="7">
-        <v>97631590</v>
+        <v>44098320</v>
       </c>
       <c r="I7" s="6">
-        <v>194890960</v>
+        <v>194644340</v>
       </c>
       <c r="J7" s="7">
-        <v>98195108</v>
+        <v>44238020</v>
       </c>
       <c r="K7" s="6">
-        <v>194810000</v>
+        <v>194726400</v>
       </c>
       <c r="L7" s="7">
-        <v>98162894</v>
+        <v>44256420</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" si="0"/>
-        <v>194528884</v>
+        <v>194553744</v>
       </c>
       <c r="N7" s="8">
         <f t="shared" ref="N7:N9" si="2">AVERAGE(D7,F7,H7,J7,L7)</f>
-        <v>98024020.799999997</v>
+        <v>44217150</v>
       </c>
       <c r="O7" s="3">
         <f t="shared" si="1"/>
-        <v>1.9845021905079823</v>
+        <v>4.3999611915286261</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
@@ -6016,46 +6016,46 @@
         <v>300000</v>
       </c>
       <c r="C8" s="6">
-        <v>565252820</v>
+        <v>568936940</v>
       </c>
       <c r="D8" s="7">
-        <v>285965820</v>
+        <v>129305570</v>
       </c>
       <c r="E8" s="6">
-        <v>565051960</v>
+        <v>566506380</v>
       </c>
       <c r="F8" s="7">
-        <v>285860350</v>
+        <v>128752770</v>
       </c>
       <c r="G8" s="6">
-        <v>568299380</v>
+        <v>565739680</v>
       </c>
       <c r="H8" s="7">
-        <v>287496520</v>
+        <v>128578970</v>
       </c>
       <c r="I8" s="6">
-        <v>565555320</v>
+        <v>565921840</v>
       </c>
       <c r="J8" s="7">
-        <v>286109916</v>
+        <v>128620170</v>
       </c>
       <c r="K8" s="6">
-        <v>567132280</v>
+        <v>566620780</v>
       </c>
       <c r="L8" s="7">
-        <v>286915840</v>
+        <v>128779720</v>
       </c>
       <c r="M8" s="6">
         <f t="shared" si="0"/>
-        <v>566258352</v>
+        <v>566745124</v>
       </c>
       <c r="N8" s="8">
         <f t="shared" si="2"/>
-        <v>286469689.19999999</v>
+        <v>128807440</v>
       </c>
       <c r="O8" s="3">
         <f t="shared" si="1"/>
-        <v>1.9766780687385896</v>
+        <v>4.3999409040347359</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
@@ -6063,46 +6063,46 @@
         <v>500000</v>
       </c>
       <c r="C9" s="6">
-        <v>930173860</v>
+        <v>929984880</v>
       </c>
       <c r="D9" s="7">
-        <v>469699456</v>
+        <v>211363520</v>
       </c>
       <c r="E9" s="6">
-        <v>929567760</v>
+        <v>930845520</v>
       </c>
       <c r="F9" s="7">
-        <v>469385888</v>
+        <v>211559470</v>
       </c>
       <c r="G9" s="6">
-        <v>930812520</v>
+        <v>928468860</v>
       </c>
       <c r="H9" s="7">
-        <v>470023520</v>
+        <v>211019520</v>
       </c>
       <c r="I9" s="6">
-        <v>932842680</v>
+        <v>928998180</v>
       </c>
       <c r="J9" s="7">
-        <v>471025892</v>
+        <v>211139520</v>
       </c>
       <c r="K9" s="6">
-        <v>930068920</v>
+        <v>931036040</v>
       </c>
       <c r="L9" s="7">
-        <v>469635602</v>
+        <v>211602570</v>
       </c>
       <c r="M9" s="6">
         <f>AVERAGE(C9,E9,G9,I9,K9)</f>
-        <v>930693148</v>
+        <v>929866696</v>
       </c>
       <c r="N9" s="8">
         <f t="shared" si="2"/>
-        <v>469954071.60000002</v>
+        <v>211336920</v>
       </c>
       <c r="O9" s="3">
         <f t="shared" si="1"/>
-        <v>1.9803917111120524</v>
+        <v>4.3999254649873762</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
@@ -6186,46 +6186,46 @@
         <v>14</v>
       </c>
       <c r="C14" s="6">
-        <v>335940</v>
+        <v>334840</v>
       </c>
       <c r="D14" s="7">
-        <v>177524</v>
+        <v>76070</v>
       </c>
       <c r="E14" s="6">
-        <v>338140</v>
+        <v>334840</v>
       </c>
       <c r="F14" s="7">
-        <v>178976</v>
+        <v>76070</v>
       </c>
       <c r="G14" s="6">
-        <v>334180</v>
+        <v>336380</v>
       </c>
       <c r="H14" s="7">
-        <v>176690</v>
+        <v>76420</v>
       </c>
       <c r="I14" s="6">
-        <v>335060</v>
+        <v>335720</v>
       </c>
       <c r="J14" s="7">
-        <v>176956</v>
+        <v>76270</v>
       </c>
       <c r="K14" s="6">
-        <v>333740</v>
+        <v>340780</v>
       </c>
       <c r="L14" s="7">
-        <v>176584</v>
+        <v>77420</v>
       </c>
       <c r="M14" s="6">
         <f>AVERAGE(C14,E14,G14,I14,K14)</f>
-        <v>335412</v>
+        <v>336512</v>
       </c>
       <c r="N14" s="8">
         <f>AVERAGE(D14,F14,H14,J14,L14)</f>
-        <v>177346</v>
+        <v>76450</v>
       </c>
       <c r="O14" s="3">
         <f t="shared" ref="O14:O19" si="3">M14/N14</f>
-        <v>1.8912859607772377</v>
+        <v>4.4017266187050357</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
@@ -6233,46 +6233,46 @@
         <v>15</v>
       </c>
       <c r="C15" s="6">
-        <v>3307040</v>
+        <v>3302640</v>
       </c>
       <c r="D15" s="7">
-        <v>1709954</v>
+        <v>750570</v>
       </c>
       <c r="E15" s="6">
-        <v>3297800</v>
+        <v>3309680</v>
       </c>
       <c r="F15" s="7">
-        <v>1703300</v>
+        <v>752220</v>
       </c>
       <c r="G15" s="6">
-        <v>3307920</v>
+        <v>3308140</v>
       </c>
       <c r="H15" s="7">
-        <v>1711780</v>
+        <v>751820</v>
       </c>
       <c r="I15" s="6">
-        <v>3297360</v>
+        <v>3302640</v>
       </c>
       <c r="J15" s="7">
-        <v>1704026</v>
+        <v>750570</v>
       </c>
       <c r="K15" s="6">
-        <v>3301760</v>
+        <v>3306160</v>
       </c>
       <c r="L15" s="7">
-        <v>1706386</v>
+        <v>751370</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" ref="M15:N19" si="4">AVERAGE(C15,E15,G15,I15,K15)</f>
-        <v>3302376</v>
+        <v>3305852</v>
       </c>
       <c r="N15" s="8">
         <f t="shared" si="4"/>
-        <v>1707089.2</v>
+        <v>751310</v>
       </c>
       <c r="O15" s="3">
         <f t="shared" si="3"/>
-        <v>1.9345069958851595</v>
+        <v>4.4001171287484526</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
@@ -6280,46 +6280,46 @@
         <v>16</v>
       </c>
       <c r="C16" s="6">
-        <v>12787280</v>
+        <v>12809280</v>
       </c>
       <c r="D16" s="7">
-        <v>6520150</v>
+        <v>2911220</v>
       </c>
       <c r="E16" s="6">
-        <v>12807740</v>
+        <v>12802900</v>
       </c>
       <c r="F16" s="7">
-        <v>6534138</v>
+        <v>2909820</v>
       </c>
       <c r="G16" s="6">
-        <v>12797180</v>
+        <v>12808180</v>
       </c>
       <c r="H16" s="7">
-        <v>6527276</v>
+        <v>2911120</v>
       </c>
       <c r="I16" s="6">
-        <v>12811920</v>
+        <v>12811480</v>
       </c>
       <c r="J16" s="7">
-        <v>6534966</v>
+        <v>2911820</v>
       </c>
       <c r="K16" s="6">
-        <v>12815660</v>
+        <v>12805100</v>
       </c>
       <c r="L16" s="7">
-        <v>6536680</v>
+        <v>2910420</v>
       </c>
       <c r="M16" s="6">
         <f t="shared" si="4"/>
-        <v>12803956</v>
+        <v>12807388</v>
       </c>
       <c r="N16" s="8">
         <f t="shared" si="4"/>
-        <v>6530642</v>
+        <v>2910880</v>
       </c>
       <c r="O16" s="3">
         <f t="shared" si="3"/>
-        <v>1.9605968295306955</v>
+        <v>4.3998337272577368</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
@@ -6327,46 +6327,46 @@
         <v>17</v>
       </c>
       <c r="C17" s="6">
-        <v>155694220</v>
+        <v>155650000</v>
       </c>
       <c r="D17" s="7">
-        <v>78820278</v>
+        <v>35375570</v>
       </c>
       <c r="E17" s="6">
-        <v>155672000</v>
+        <v>155700160</v>
       </c>
       <c r="F17" s="7">
-        <v>78806278</v>
+        <v>35386620</v>
       </c>
       <c r="G17" s="6">
-        <v>155657920</v>
+        <v>155669800</v>
       </c>
       <c r="H17" s="7">
-        <v>78801702</v>
+        <v>35379770</v>
       </c>
       <c r="I17" s="6">
-        <v>155633940</v>
+        <v>155677500</v>
       </c>
       <c r="J17" s="7">
-        <v>78789914</v>
+        <v>35381520</v>
       </c>
       <c r="K17" s="6">
-        <v>155663860</v>
+        <v>155656380</v>
       </c>
       <c r="L17" s="7">
-        <v>78808074</v>
+        <v>35376970</v>
       </c>
       <c r="M17" s="6">
         <f t="shared" si="4"/>
-        <v>155664388</v>
+        <v>155670768</v>
       </c>
       <c r="N17" s="8">
         <f t="shared" si="4"/>
-        <v>78805249.200000003</v>
+        <v>35380090</v>
       </c>
       <c r="O17" s="3">
         <f t="shared" si="3"/>
-        <v>1.9753048125631711</v>
+        <v>4.3999539854194829</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
@@ -6374,46 +6374,46 @@
         <v>18</v>
       </c>
       <c r="C18" s="6">
-        <v>777536320</v>
+        <v>777566240</v>
       </c>
       <c r="D18" s="7">
-        <v>392519164</v>
+        <v>176721320</v>
       </c>
       <c r="E18" s="6">
-        <v>777586700</v>
+        <v>777605180</v>
       </c>
       <c r="F18" s="7">
-        <v>392550712</v>
+        <v>176731170</v>
       </c>
       <c r="G18" s="6">
-        <v>777588240</v>
+        <v>777536980</v>
       </c>
       <c r="H18" s="7">
-        <v>392546706</v>
+        <v>176715670</v>
       </c>
       <c r="I18" s="6">
+        <v>777553480</v>
+      </c>
+      <c r="J18" s="7">
+        <v>176718370</v>
+      </c>
+      <c r="K18" s="6">
         <v>777557880</v>
       </c>
-      <c r="J18" s="7">
-        <v>392528884</v>
-      </c>
-      <c r="K18" s="6">
-        <v>777554140</v>
-      </c>
       <c r="L18" s="7">
-        <v>392532252</v>
+        <v>176720170</v>
       </c>
       <c r="M18" s="6">
         <f t="shared" si="4"/>
-        <v>777564656</v>
+        <v>777563952</v>
       </c>
       <c r="N18" s="8">
         <f t="shared" si="4"/>
-        <v>392535543.60000002</v>
+        <v>176721340</v>
       </c>
       <c r="O18" s="3">
         <f t="shared" si="3"/>
-        <v>1.9808770662367094</v>
+        <v>4.3999437306213274</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
@@ -6421,46 +6421,46 @@
         <v>19</v>
       </c>
       <c r="C19" s="6">
-        <v>1828519660</v>
+        <v>1828554640</v>
       </c>
       <c r="D19" s="7">
-        <v>919383068</v>
+        <v>415586670</v>
       </c>
       <c r="E19" s="6">
-        <v>1828465760</v>
+        <v>1828473460</v>
       </c>
       <c r="F19" s="7">
-        <v>919329658</v>
+        <v>415567920</v>
       </c>
       <c r="G19" s="6">
-        <v>1828424180</v>
+        <v>1828524720</v>
       </c>
       <c r="H19" s="7">
-        <v>919323052</v>
+        <v>415578720</v>
       </c>
       <c r="I19" s="6">
-        <v>1828424620</v>
+        <v>1828429020</v>
       </c>
       <c r="J19" s="7">
-        <v>919323558</v>
+        <v>415556570</v>
       </c>
       <c r="K19" s="6">
-        <v>1828494360</v>
+        <v>1828579720</v>
       </c>
       <c r="L19" s="7">
-        <v>919366178</v>
+        <v>415592520</v>
       </c>
       <c r="M19" s="6">
         <f t="shared" si="4"/>
-        <v>1828465716</v>
+        <v>1828512312</v>
       </c>
       <c r="N19" s="8">
         <f t="shared" si="4"/>
-        <v>919345102.79999995</v>
+        <v>415576480</v>
       </c>
       <c r="O19" s="3">
         <f t="shared" si="3"/>
-        <v>1.9888785075714661</v>
+        <v>4.3999417676380528</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">

</xml_diff>